<commit_message>
update tp biochimie ~Raphael 19h34 13-11-20
</commit_message>
<xml_diff>
--- a/Excel/UV1.xlsx
+++ b/Excel/UV1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\VirtualBox VMs\SciViews Box 2020\shared\projects\TP-Bioch-BAB2-Q1\Dataframes Excel (.xlsx)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafde\VirtualBox VMs\SciViews Box 2020\shared\projects\TP-Bioch-BAB2-Q1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26ADFF18-206B-4BE1-8010-04BF0FCCBAD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68893E4-6C5D-4C11-9275-A0EA99CAFDE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6345" yWindow="2955" windowWidth="21600" windowHeight="11385" xr2:uid="{8E9AD17E-C068-41C7-8AC5-D3F2EA617C1C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E9AD17E-C068-41C7-8AC5-D3F2EA617C1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Longueur d'onde</t>
+  </si>
+  <si>
+    <t>Absorbance de la solution diluée x100</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,12 +390,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB65F22-CC3A-464D-AA4B-F6FFE65CBC4D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>250</v>
+      </c>
+      <c r="B2">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>260</v>
+      </c>
+      <c r="B3">
+        <v>0.185</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>270</v>
+      </c>
+      <c r="B4">
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>280</v>
+      </c>
+      <c r="B5">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>290</v>
+      </c>
+      <c r="B6">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>300</v>
+      </c>
+      <c r="B7">
+        <v>3.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>310</v>
+      </c>
+      <c r="B8">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>320</v>
+      </c>
+      <c r="B9">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>330</v>
+      </c>
+      <c r="B10">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>340</v>
+      </c>
+      <c r="B11">
+        <v>-1.2E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>350</v>
+      </c>
+      <c r="B12">
+        <v>-1.2E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>